<commit_message>
converted summer progress to master.
</commit_message>
<xml_diff>
--- a/StoveOpt/stovegeom/Stove_Geometry.xlsx
+++ b/StoveOpt/stovegeom/Stove_Geometry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\stovegeom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\StoveOpt\stovegeom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7CC635-7A53-47CD-9420-6D6B9D702305}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF0683-515D-4CA0-8FE1-0D7B03860B0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
   <si>
     <t>Geometry</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>m2/s</t>
-  </si>
-  <si>
-    <t>U_100</t>
   </si>
   <si>
     <t>Primary air flow rate</t>
@@ -328,7 +325,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -419,9 +416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,6 +429,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +531,7 @@
             <c:numRef>
               <c:f>Outputs!$C$2:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -591,7 +588,7 @@
             <c:numRef>
               <c:f>Outputs!$D$2:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -683,7 +680,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -745,7 +742,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1864,13 +1861,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1193722</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>137929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>299873</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>29402</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2241,7 +2238,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -2256,7 +2253,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -2271,7 +2268,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>32</v>
@@ -2286,7 +2283,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -2302,7 +2299,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -2317,7 +2314,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -2332,7 +2329,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -2347,7 +2344,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -2362,7 +2359,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
@@ -2397,7 +2394,7 @@
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2411,21 +2408,21 @@
       <c r="C14" s="3">
         <v>0.1</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2893,7 +2890,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2919,10 +2916,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -3405,8 +3402,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>47</v>
+      <c r="A20" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B20" s="1">
         <f>D6-D5</f>
@@ -3415,67 +3412,67 @@
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>58</v>
+      <c r="F20" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>48</v>
+      <c r="A21" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B21" s="1">
         <f>(PI()/4)*B20^2</f>
         <v>7.8539816339744976E-5</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="B22" s="1">
         <v>318.30988618379001</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="B23" s="1">
         <f>B22*B21</f>
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>55</v>
+      <c r="A24" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <f>1.225</f>
         <v>1.2250000000000001</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>54</v>
+      <c r="A25" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B25" s="1">
         <f>B24*B23</f>
         <v>3.0624999999999996E-2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3485,26 +3482,26 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1">
         <f>2</f>
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1">
         <f>B28/60</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3517,7 +3514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB2BEC4-1E12-4134-95E6-A4E4264AA137}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -3530,7 +3527,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1">
         <v>0.01</v>
@@ -3541,7 +3538,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <f>2*B1</f>
@@ -3550,7 +3547,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -3558,7 +3555,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -3566,7 +3563,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>2.5</v>
@@ -3574,7 +3571,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <f>B3*B2 + B5*B6</f>
@@ -3583,7 +3580,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <f>(B5/2)*2</f>
@@ -3592,7 +3589,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12">
         <f>0.03*2</f>
@@ -3601,7 +3598,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>0.25</v>
@@ -3609,7 +3606,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <f>(B11*B13)+(B12*B13)</f>
@@ -3618,37 +3615,37 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16">
         <v>0.04</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <f>B8/B14</f>
         <v>10.735586481113319</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17">
         <f>1.225</f>
         <v>1.2250000000000001</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18">
         <f>H16/H17</f>
@@ -3657,7 +3654,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19">
         <f>H18/(PI()*0.25*(0.1^2))</f>
@@ -3672,10 +3669,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3688,7 +3685,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3708,21 +3705,21 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
         <f>Intermediate!C2*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="9">
         <f>Intermediate!D2*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="9">
         <f>Intermediate!E2*(1/100)</f>
         <v>0</v>
       </c>
@@ -3731,21 +3728,21 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
         <f>Intermediate!C3*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="9">
         <f>Intermediate!D3*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="9">
         <f>Intermediate!E3*(1/100)</f>
         <v>0</v>
       </c>
@@ -3754,21 +3751,21 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
         <f>Intermediate!C4*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="9">
         <f>Intermediate!D4*(1/100)</f>
         <v>0.15</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="9">
         <f>Intermediate!E4*(1/100)</f>
         <v>0</v>
       </c>
@@ -3777,21 +3774,21 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
         <f>Intermediate!C5*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="9">
         <f>Intermediate!D5*(1/100)</f>
         <v>0.15</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="9">
         <f>Intermediate!E5*(1/100)</f>
         <v>0</v>
       </c>
@@ -3800,21 +3797,21 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
         <f>Intermediate!C6*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="9">
         <f>Intermediate!D6*(1/100)</f>
         <v>0.16</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
         <f>Intermediate!E6*(1/100)</f>
         <v>0</v>
       </c>
@@ -3823,21 +3820,21 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
         <f>Intermediate!C7*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="9">
         <f>Intermediate!D7*(1/100)</f>
         <v>0.16</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="9">
         <f>Intermediate!E7*(1/100)</f>
         <v>0</v>
       </c>
@@ -3846,21 +3843,21 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="3">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9">
         <f>Intermediate!C8*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="9">
         <f>Intermediate!D8*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="9">
         <f>Intermediate!E8*(1/100)</f>
         <v>0</v>
       </c>
@@ -3869,21 +3866,21 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
         <f>Intermediate!C9*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="9">
         <f>Intermediate!D9*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="9">
         <f>Intermediate!E9*(1/100)</f>
         <v>0</v>
       </c>
@@ -3892,21 +3889,21 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
         <f>Intermediate!C10*(1/100)</f>
         <v>0.17</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="9">
         <f>Intermediate!D10*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="9">
         <f>Intermediate!E10*(1/100)</f>
         <v>0</v>
       </c>
@@ -3915,21 +3912,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
         <f>Intermediate!C11*(1/100)</f>
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="9">
         <f>Intermediate!D11*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="9">
         <f>Intermediate!E11*(1/100)</f>
         <v>0</v>
       </c>
@@ -3938,21 +3935,21 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="3">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
         <f>Intermediate!C12*(1/100)</f>
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="9">
         <f>Intermediate!D12*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="9">
         <f>Intermediate!E12*(1/100)</f>
         <v>0</v>
       </c>
@@ -3961,21 +3958,21 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="3">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
         <f>Intermediate!C13*(1/100)</f>
         <v>-0.04</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="9">
         <f>Intermediate!D13*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="9">
         <f>Intermediate!E13*(1/100)</f>
         <v>0</v>
       </c>
@@ -3984,21 +3981,21 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="3">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9">
         <f>Intermediate!C14*(1/100)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="9">
         <f>Intermediate!D14*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="9">
         <f>Intermediate!E14*(1/100)</f>
         <v>0</v>
       </c>
@@ -4007,21 +4004,21 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="3">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9">
         <f>Intermediate!C15*(1/100)</f>
         <v>0.17</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="9">
         <f>Intermediate!D15*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="9">
         <f>Intermediate!E15*(1/100)</f>
         <v>0</v>
       </c>
@@ -4030,21 +4027,21 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="3">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9">
         <f>Intermediate!C16*(1/100)</f>
         <v>-0.04</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="9">
         <f>Intermediate!D16*(1/100)</f>
         <v>0.33</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="9">
         <f>Intermediate!E16*(1/100)</f>
         <v>0</v>
       </c>
@@ -4053,21 +4050,21 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="3">
-        <v>15</v>
-      </c>
-      <c r="C17" s="4">
+        <v>16</v>
+      </c>
+      <c r="C17" s="9">
         <f>Intermediate!C17*(1/100)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="9">
         <f>Intermediate!D17*(1/100)</f>
         <v>0.33</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="9">
         <f>Intermediate!E17*(1/100)</f>
         <v>0</v>
       </c>
@@ -4077,22 +4074,11 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3">
-        <f>ABS(Inputs!C14)</f>
-        <v>0.1</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -4142,14 +4128,6 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>